<commit_message>
Enabled copying of formulas
</commit_message>
<xml_diff>
--- a/Excel/Template.xlsx
+++ b/Excel/Template.xlsx
@@ -8,14 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bwynn\Documents\Python\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E329663-F4ED-42E7-8DAC-E82DAECEF788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C020572-EF11-42D3-8C12-FFD7632629C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="850" windowWidth="18940" windowHeight="8850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CashFlow" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -25,16 +35,15 @@
     <t>Cost</t>
   </si>
   <si>
-    <t>Cumulative Cost</t>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -117,7 +126,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -126,13 +135,13 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="-2056189179504541898" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="8667842428121483311" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -419,7 +428,7 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="30.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -435,6 +444,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
+        <f>A2/SUM(A:A)</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement writing to multiple sheets
</commit_message>
<xml_diff>
--- a/Excel/Template.xlsx
+++ b/Excel/Template.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bwynn\Documents\Python\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C020572-EF11-42D3-8C12-FFD7632629C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE0535D-541F-4091-BC9B-A9EC677ADE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="850" windowWidth="18940" windowHeight="8850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="260" yWindow="850" windowWidth="18940" windowHeight="8850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CashFlow" sheetId="1" r:id="rId1"/>
+    <sheet name="CashFlowV2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,12 +31,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Cost</t>
   </si>
   <si>
     <t>Percentage</t>
+  </si>
+  <si>
+    <t>Id Text</t>
+  </si>
+  <si>
+    <t>Id1</t>
   </si>
 </sst>
 </file>
@@ -128,7 +135,7 @@
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -136,6 +143,8 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="-2056189179504541898" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -421,7 +430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -452,4 +461,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34AAC7BB-5862-41DE-8DF3-B635A1977160}">
+  <dimension ref="A2:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.54296875" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>